<commit_message>
Update Feb 6 2014
</commit_message>
<xml_diff>
--- a/projFocus/ceRNA/doc/modelCases.xlsx
+++ b/projFocus/ceRNA/doc/modelCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
   <si>
     <t>snp</t>
   </si>
@@ -102,7 +102,10 @@
     <t>case 16</t>
   </si>
   <si>
-    <t>ftest Model</t>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
       <name val="Zapf Dingbats"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +186,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -193,7 +202,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -269,10 +278,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,18 +313,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -344,6 +377,11 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -381,11 +419,202 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Zapf Dingbats"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Zapf Dingbats"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Zapf Dingbats"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Zapf Dingbats"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Zapf Dingbats"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1651000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7251700" y="0"/>
+          <a:ext cx="5613400" cy="3352800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I17" totalsRowShown="0" headerRowDxfId="7">
+  <tableColumns count="9">
+    <tableColumn id="1" name="Model" dataDxfId="6"/>
+    <tableColumn id="2" name="exp" dataDxfId="5"/>
+    <tableColumn id="3" name="snp" dataDxfId="4"/>
+    <tableColumn id="4" name="indel" dataDxfId="3"/>
+    <tableColumn id="5" name="som" dataDxfId="2"/>
+    <tableColumn id="6" name="cnv" dataDxfId="0"/>
+    <tableColumn id="7" name="Column1" dataDxfId="1"/>
+    <tableColumn id="8" name="Model Number"/>
+    <tableColumn id="9" name="progress"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -713,58 +942,62 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:J17"/>
+      <selection sqref="A1:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="0" style="8" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -776,49 +1009,49 @@
       <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="11"/>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -827,303 +1060,331 @@
       <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="7" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="7" t="s">
+    <row r="12" spans="1:13">
+      <c r="A12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="7" t="s">
+    <row r="13" spans="1:13">
+      <c r="A13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B15" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="12" t="s">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>